<commit_message>
correct fetch api page produit
</commit_message>
<xml_diff>
--- a/Template+de+Plan+de+tests.xlsx
+++ b/Template+de+Plan+de+tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\JWDP5-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE949EB0-C146-477A-A55C-893D8500B691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C503ACFE-9C07-4E2E-B40B-82DF221C6ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1500" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -79,12 +79,6 @@
     <t>4 à 13</t>
   </si>
   <si>
-    <t>19à 68</t>
-  </si>
-  <si>
-    <t>71 à 88</t>
-  </si>
-  <si>
     <t>5 à 44</t>
   </si>
   <si>
@@ -1012,6 +1006,12 @@
 Il faut empêcher une commande sans produit.
 Le back-end ne renvoie pas le bon prix de la commande à cause de la quantité.</t>
     </r>
+  </si>
+  <si>
+    <t>19à 85</t>
+  </si>
+  <si>
+    <t>70 à 83</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1194,16 +1194,19 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1427,8 +1430,8 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1459,7 +1462,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1482,44 +1485,44 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:26" s="12" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>28</v>
+    </row>
+    <row r="3" spans="1:26" s="12" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
+      <c r="E3" s="11" t="s">
+        <v>30</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1533,53 +1536,53 @@
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:26" s="12" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>19</v>
+      <c r="B5" s="10" t="s">
+        <v>47</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="10" t="s">
+    </row>
+    <row r="6" spans="1:26" s="12" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="E6" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
@@ -1587,19 +1590,19 @@
         <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="90" customHeight="1" x14ac:dyDescent="0.2">
@@ -1607,19 +1610,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1627,19 +1630,19 @@
         <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>